<commit_message>
Update lại Final Report Tasksheet.xlsx #LongDB
</commit_message>
<xml_diff>
--- a/wiki/report/Final Report Tasksheet.xlsx
+++ b/wiki/report/Final Report Tasksheet.xlsx
@@ -439,6 +439,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -451,20 +463,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,20 +772,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="8.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
@@ -813,7 +813,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="20"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="10"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -823,7 +823,7 @@
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A3" s="19"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="13"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -833,7 +833,7 @@
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A4" s="19"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="13"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -843,7 +843,7 @@
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="13"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -853,7 +853,7 @@
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A6" s="19"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="13"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -863,7 +863,7 @@
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="13"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -873,7 +873,7 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="13"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -883,7 +883,7 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="13"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -893,7 +893,7 @@
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="13"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -903,7 +903,7 @@
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A11" s="19"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="13"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -913,7 +913,7 @@
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" hidden="1" customHeight="1">
-      <c r="A12" s="19"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="13"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -923,7 +923,7 @@
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -939,7 +939,7 @@
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
-      <c r="A14" s="22"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="18" t="s">
         <v>9</v>
       </c>
@@ -957,7 +957,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -973,7 +973,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
-      <c r="A16" s="19"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75">
-      <c r="A17" s="19"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="8" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1009,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75">
-      <c r="A18" s="19"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="15.75">
-      <c r="A19" s="19"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75">
-      <c r="A20" s="19"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="15.75">
-      <c r="A21" s="19"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="8" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75">
-      <c r="A23" s="25"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="18" t="s">
         <v>26</v>
       </c>
@@ -1111,7 +1111,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75">
-      <c r="A24" s="25"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="18" t="s">
         <v>27</v>
       </c>
@@ -1129,8 +1129,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="27"/>
+      <c r="B25" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="7"/>
@@ -1145,7 +1145,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75">
-      <c r="A26" s="25"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="18" t="s">
         <v>29</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75">
-      <c r="A27" s="25"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="18" t="s">
         <v>30</v>
       </c>
@@ -1181,8 +1181,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="25"/>
-      <c r="B28" s="27" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7"/>
@@ -1199,14 +1199,14 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75">
-      <c r="A29" s="25"/>
-      <c r="B29" s="27" t="s">
+      <c r="A29" s="27"/>
+      <c r="B29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="17">
@@ -1217,14 +1217,14 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75">
-      <c r="A30" s="25"/>
-      <c r="B30" s="27" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="7"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="17">
@@ -1235,14 +1235,14 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75">
-      <c r="A31" s="25"/>
-      <c r="B31" s="27" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="7"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="17">
@@ -1253,14 +1253,14 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75">
-      <c r="A32" s="25"/>
-      <c r="B32" s="27" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="7"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="7" t="s">
+        <v>0</v>
+      </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="17">
@@ -1271,14 +1271,14 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75">
-      <c r="A33" s="25"/>
-      <c r="B33" s="27" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C33" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="17">
@@ -1289,14 +1289,14 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75">
-      <c r="A34" s="25"/>
-      <c r="B34" s="27" t="s">
+      <c r="A34" s="27"/>
+      <c r="B34" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="17">
@@ -1307,14 +1307,14 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75">
-      <c r="A35" s="25"/>
-      <c r="B35" s="27" t="s">
+      <c r="A35" s="27"/>
+      <c r="B35" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="17">
@@ -1333,7 +1333,7 @@
     <mergeCell ref="A22:A35"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F35 D29:D32 C2:D28 C33:C35">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>